<commit_message>
rework tracks torque/speed averaging handling, now seems to perform appropriately
</commit_message>
<xml_diff>
--- a/TrackTorque.xlsx
+++ b/TrackTorque.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_source\git\KSPWheel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19890" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>wheel radius</t>
   </si>
@@ -65,9 +60,6 @@
     <t>total t</t>
   </si>
   <si>
-    <t>w out</t>
-  </si>
-  <si>
     <t>v</t>
   </si>
   <si>
@@ -77,22 +69,31 @@
     <t>total r</t>
   </si>
   <si>
-    <t>v out</t>
-  </si>
-  <si>
-    <t>sharSum</t>
-  </si>
-  <si>
     <t>tshare</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>totalMOI</t>
   </si>
   <si>
-    <t>torqueSum</t>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>share</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>torque input</t>
+  </si>
+  <si>
+    <t>in share</t>
+  </si>
+  <si>
+    <t>w a</t>
+  </si>
+  <si>
+    <t>new v</t>
   </si>
 </sst>
 </file>
@@ -134,7 +135,78 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -402,7 +474,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -410,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,6 +496,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -535,7 +608,7 @@
         <v>2976.1904761904757</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L5" si="6">K3*A3</f>
+        <f t="shared" ref="L3:L4" si="6">K3*A3</f>
         <v>595.23809523809518</v>
       </c>
     </row>
@@ -610,25 +683,25 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
         <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" t="s">
         <v>13</v>
-      </c>
-      <c r="K10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -653,15 +726,15 @@
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G11">
-        <f xml:space="preserve"> (A11 / $E$18) * $E$16</f>
-        <v>1.4999999999999998E-3</v>
+        <f>C11/A11</f>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H11">
-        <f>G11/$E$16</f>
+        <f>G11/$G$14</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="I11">
-        <f>H11*$E$16</f>
+        <f>H11*$F$14</f>
         <v>1.4999999999999998E-3</v>
       </c>
       <c r="J11">
@@ -672,10 +745,6 @@
         <f>J11*A11</f>
         <v>0.375</v>
       </c>
-      <c r="L11">
-        <f>A11/$E$18*$E$16</f>
-        <v>1.4999999999999998E-3</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -699,15 +768,15 @@
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="G12">
-        <f t="shared" ref="G12:G13" si="8" xml:space="preserve"> (A12 / $E$18) * $E$16</f>
-        <v>2.9999999999999996E-3</v>
+        <f>C12/A12</f>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H12">
-        <f t="shared" ref="H12:H13" si="9">G12/$E$16</f>
+        <f>G12/$G$14</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="I12">
-        <f t="shared" ref="I12:I13" si="10">H12*$E$16</f>
+        <f t="shared" ref="I12:I13" si="8">H12*$F$14</f>
         <v>2.9999999999999996E-3</v>
       </c>
       <c r="J12">
@@ -718,10 +787,6 @@
         <f>J12*A12</f>
         <v>0.375</v>
       </c>
-      <c r="L12">
-        <f t="shared" ref="L12:L13" si="11">A12/$E$18*$E$16</f>
-        <v>2.9999999999999996E-3</v>
-      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -745,28 +810,24 @@
         <v>7.1999999999999998E-3</v>
       </c>
       <c r="G13">
+        <f>C13/A13</f>
+        <v>1.2E-2</v>
+      </c>
+      <c r="H13">
+        <f>G13/$G$14</f>
+        <v>0.5</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="8"/>
-        <v>4.4999999999999988E-3</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="9"/>
-        <v>0.49999999999999989</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="10"/>
-        <v>4.4999999999999988E-3</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="J13">
         <f>I13/C13</f>
-        <v>1.2499999999999998</v>
+        <v>1.25</v>
       </c>
       <c r="K13">
         <f>J13*A13</f>
-        <v>0.37499999999999994</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="11"/>
-        <v>4.4999999999999988E-3</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -774,21 +835,38 @@
         <f>SUM(E11:E13)/COUNT(E11:E13)</f>
         <v>0.28333333333333333</v>
       </c>
-      <c r="G14" t="s">
-        <v>18</v>
+      <c r="F14">
+        <f>SUM(F11:F13)</f>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G14">
+        <f>SUM(G11:G13)</f>
+        <v>2.4E-2</v>
       </c>
       <c r="H14">
-        <f>SUM(H11:H13)</f>
-        <v>0.99999999999999989</v>
+        <f t="shared" ref="H14:I14" si="9">SUM(H11:H13)</f>
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="9"/>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="L14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15">
-        <f>SUM(G11:G13)</f>
-        <v>8.9999999999999976E-3</v>
+      <c r="H15" t="b">
+        <f>H14=1</f>
+        <v>1</v>
+      </c>
+      <c r="I15" t="b">
+        <f>I14=F14</f>
+        <v>1</v>
+      </c>
+      <c r="K15" t="b">
+        <f>K13=K12=K11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -800,34 +878,245 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17">
         <f>SUM(E11:E13)</f>
         <v>0.85</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18">
         <f>SUM(A11:A13)</f>
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E19">
         <f>SUM(C11:C13)</f>
         <v>5.5999999999999999E-3</v>
       </c>
     </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.1</v>
+      </c>
+      <c r="B23">
+        <v>0.04</v>
+      </c>
+      <c r="C23">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D23">
+        <v>3.75</v>
+      </c>
+      <c r="E23">
+        <f>D23*A23</f>
+        <v>0.375</v>
+      </c>
+      <c r="F23">
+        <f>D23*C23</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="G23">
+        <f>C23/A23</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H23">
+        <f>G23/$G$26</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I23">
+        <f>H23*$B$21</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J23">
+        <f>I23/C23</f>
+        <v>833.33333333333326</v>
+      </c>
+      <c r="K23">
+        <f>(J23*A23) +E23</f>
+        <v>83.708333333333329</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.2</v>
+      </c>
+      <c r="B24">
+        <v>0.04</v>
+      </c>
+      <c r="C24">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D24">
+        <v>1.875</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E24:E25" si="10">D24*A24</f>
+        <v>0.375</v>
+      </c>
+      <c r="F24">
+        <f>D24*C24</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G24">
+        <f>C24/A24</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ref="H24:H25" si="11">G24/$G$26</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I24">
+        <f t="shared" ref="I24:I25" si="12">H24*$B$21</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J24">
+        <f>I24/C24</f>
+        <v>416.66666666666663</v>
+      </c>
+      <c r="K24">
+        <f>(J24*A24) +E24</f>
+        <v>83.708333333333329</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.3</v>
+      </c>
+      <c r="B25">
+        <v>0.04</v>
+      </c>
+      <c r="C25">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="D25">
+        <v>1.25</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="10"/>
+        <v>0.375</v>
+      </c>
+      <c r="F25">
+        <f>D25*C25</f>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="G25">
+        <f>C25/A25</f>
+        <v>1.2E-2</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="11"/>
+        <v>0.5</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <f>I25/C25</f>
+        <v>277.77777777777777</v>
+      </c>
+      <c r="K25">
+        <f>(J25*A25) +E25</f>
+        <v>83.708333333333329</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f>SUM(F23:F25)</f>
+        <v>9.0000000000000011E-3</v>
+      </c>
+      <c r="G26">
+        <f>SUM(G23:G25)</f>
+        <v>2.4E-2</v>
+      </c>
+      <c r="H26">
+        <f t="shared" ref="H26:I26" si="13">SUM(H23:H25)</f>
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H27" t="b">
+        <f>H26=1</f>
+        <v>1</v>
+      </c>
+      <c r="I27" t="b">
+        <f>I26=B21</f>
+        <v>1</v>
+      </c>
+      <c r="K27" t="b">
+        <f>AND(K23=K24,K24=K25)</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="H15:K15">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27:K27">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>